<commit_message>
feat: Make sidebar non-fixed and allow full-width content when collapsed
- Updated sidebar styling to remove fixed positioning
- Added CSS transitions for smooth sidebar toggle animations
- Enhanced dashboard layout to use flexbox for responsive content expansion
- Improved form handling with proper validation and success messaging
- Added dynamic data saving to persistent storage
</commit_message>
<xml_diff>
--- a/data/cpms_data.xlsx
+++ b/data/cpms_data.xlsx
@@ -716,7 +716,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,11 +815,65 @@
           <t>asdfg</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>21321</v>
-      </c>
-      <c r="J2" t="n">
-        <v>213123</v>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>21321</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>213123</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Registered</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>REGION XI (DAVAO REGION)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>DAVAO DEL SUR</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>DAVAO CITY</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Acacia</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>21344tytr3</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1435y643524</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4324577i76543</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>esadfdgghhjgfsd</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comprehensive delete functionality and form enhancements
- Implemented delete row functionality with dropdown selection
- Added delete all rows feature with confirmation
- Created undo system for both delete operations
- Enhanced all 14 sheet forms with proper validation
- Added PSIC classification system with cascading dropdowns
- Integrated location widgets across all relevant forms
- Added date pickers with MM/DD/YYYY formatting
- Improved form state management and success messaging
- Added comprehensive field validation (required vs optional)
- Enhanced user experience with standardized data entry
</commit_message>
<xml_diff>
--- a/data/cpms_data.xlsx
+++ b/data/cpms_data.xlsx
@@ -7,18 +7,19 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Business Financial Structure" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Client" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Business Contact Information" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Business Registrations" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Business Owner" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Business Profile" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Market Import" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Jobs Generated" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Assistance" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Market Domestic" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Market Export" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Product_Service Lines" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Product Service Lines" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Business Contact Information" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Business Owner" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Jobs Generated" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Assistance" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Employment Statistics" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Business Registrations" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Business Profile" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Market Import" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Market Export" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Market Domestic" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Business Financial Structure" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Client" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,22 +453,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Asset Classification Year</t>
+          <t>Product/Service Line</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Asset Size Range</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Sales History Year</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Domestic Sales</t>
+          <t>Major Raw Material/s</t>
         </is>
       </c>
     </row>
@@ -477,47 +468,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Product/Service</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Region</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Province</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -544,17 +494,102 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Product Service</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Trade Bloc</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Product/Service</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Trade Bloc</t>
+          <t>Province</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>shabu</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>REGION I (ILOCOS REGION)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ILOCOS NORTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mariwana</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>REGION XI (DAVAO REGION)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>DAVAO DEL SUR</t>
         </is>
       </c>
     </row>
@@ -569,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,12 +620,335 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Product/Service Line</t>
+          <t>Initial Capitalization</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Major Raw Material/s</t>
+          <t>Capital Structure</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Authorize Capital</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Subscribed Capital</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Paid Up Capital</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Capitalization Year</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Asset Classification Year</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Asset Size Range</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Sales History Year</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Domestic Sales</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Export Sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>hahaha</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>aaaaaaa</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date Created (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status of Client</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Specify Level 1.1 and 1.2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Category of Client</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Social Classification</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Diff/Abled Type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Client is Senior</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Client is Indigenous</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Level of Digitalization</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Digital Tools</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>MSME Classification</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Client Designation</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Middle Name</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Suffix</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Civil Status</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Barangay</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Landline Number</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Fax Number</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Mobile Number</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Email Address</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Social Media</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>E-Commerce Platform</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>08/08/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Level 0 - Would be or Potential Entrepreneurs</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Self-Employed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Abled</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Level 0 - No use of digital tools</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Owner</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>asasd</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>ase21sad</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>hahaha</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>123213</t>
         </is>
       </c>
     </row>
@@ -605,7 +963,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,87 +979,159 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Date Created (MM/DD/YYYY)</t>
+          <t>Status of Business Registration</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Status of Client</t>
+          <t>Registered Business</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Category of Client</t>
+          <t>Date Registered (MM/DD/YYYY)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Social Classification</t>
+          <t>Business Company Name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Client is Senior</t>
+          <t>Trade or Billboard Name</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Client is Indigenous</t>
+          <t>IPO Registration Number</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Level of Digitalization</t>
+          <t>Region</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Client Designation</t>
+          <t>Province</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>City/Municipality</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Barangay</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Civil Status</t>
+          <t>District</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Zip Code</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Barangay</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>District</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>Landline Number</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Fax Number</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Mobile Number</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Email Address</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>E-Commerce Platform</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Social Media</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Third Party Platform</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Registered</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>REGION I (ILOCOS REGION)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ILOCOS NORTE</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>ADAMS</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Adams (Pob.)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>12341</t>
         </is>
       </c>
     </row>
@@ -716,7 +1146,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,147 +1162,174 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Status of Business Registration</t>
+          <t>Given Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Middle Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Suffix</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Civil Status</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Birthdate (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Birth Year</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Citizenship</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Social Classification</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Diff/Abled type</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Owner is Senior</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Owner is Indigenous</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Province</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>City/Municipality</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Barangay</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>District</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Mobile Number</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Email Address</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Registered</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>REGION III (CENTRAL LUZON)</t>
+          <t>aaaaaa</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BATAAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ABUCAY</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Bangkal</t>
+          <t>Single</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>sadgd</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>asdfg</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>21321</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>213123</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Registered</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+          <t>Filipino</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Abled</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>REGION XI (DAVAO REGION)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>DAVAO DEL SUR</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DAVAO CITY</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Acacia</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>21344tytr3</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1435y643524</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>4324577i76543</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>esadfdgghhjgfsd</t>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>DAVAO DEL NORTE</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>ASUNCION (SAUG)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Binancian</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>hahaha</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>erwqrawhadfas</t>
         </is>
       </c>
     </row>
@@ -887,7 +1344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,22 +1360,79 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name of Business</t>
+          <t>Date Recorded (MM/DD/YYYY)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Registering Agency</t>
+          <t>Direct Community Jobs</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Agency Expiry Date (MM/DD/YYYY)</t>
+          <t>Indirect Community Jobs</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Agency Reg Number</t>
+          <t>Direct Home Based</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Indirect Home Based</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Direct Jobs Sustained</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Indirect Jobs Sustained</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>08/08/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ahahah</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>haha</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>hahaha</t>
         </is>
       </c>
     </row>
@@ -933,7 +1447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -949,72 +1463,219 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Given Name</t>
+          <t>EDT Assistance Level</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Type of Assistance</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Civil Status</t>
+          <t>Sub Type of Assistance</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Sex</t>
+          <t>Remarks</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Citizenship</t>
+          <t>Date Start (MM/DD/YYYY)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Social Classification</t>
+          <t>Date End (MM/DD/YYYY)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Owner is Senior</t>
+          <t>MSME Program</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Owner is Indigenous</t>
+          <t>MSME Availed (MM/DD/YYYY)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Region</t>
+          <t>Assisted By</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Province</t>
+          <t>Assisting Office</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>City/Municipality</t>
+          <t>Type of NC</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Barangay</t>
+          <t>Location of NC</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>District</t>
+          <t>Assisting Officer Region</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Assisting Officer Province</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Assisting Officer City</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Jobs Generated</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Investment Generated</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Domestic Sales Generated</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Export Sales Generated</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Amount Loan Grant</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Fund Source</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Abled Male</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Abled Female</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Training – PWD Male</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Training – PWD Female</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Indigenous Male</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Indigenous Female</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Senior Male</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Training – Senior Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Level 0 - Entrepreneurial Mind Setting</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BN Registration</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>hahaha</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>08/20/2026</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Negosyo Center</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>08/06/2025</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Analiza Montero</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Negosyo Center</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>REGION XI (DAVAO REGION)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>DAVAO DEL SUR</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>DAVAO CITY</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,42 +1706,355 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Year Established</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Form of Organization</t>
+          <t>Fulltime Abled Male</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Major Activity</t>
+          <t>Fulltime Abled Female</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Minor Activity</t>
+          <t>Fulltime PWD Male</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>PSIC Group</t>
+          <t>Fulltime PWD Female</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>PSIC Division</t>
+          <t>Fulltime Indigenous Male</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>PSIC Section</t>
+          <t>Fulltime Indigenous Female</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Prio Industry Cluster</t>
+          <t>Fulltime Senior Male</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Fulltime Senior Female</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time Abled Male</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time Abled Female</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time PWD Male</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time PWD Female</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time Indigenous Male</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time Indigenous Female</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time Senior Male</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Part-time Senior Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1095,7 +2069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,17 +2085,104 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Year Import Started</t>
+          <t>Name of Business</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Product Service</t>
+          <t>Registering Agency</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Agency Expiry Date (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Agency Reg Number</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Business Permit</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Bus Permit Expiry Date (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bus Permit Reg Number</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BIR (TIN) No.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>BMBE Registration</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>BMBE Expiry Date (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>FDA Reg Number</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>FDA Expiry Date (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Certification Type</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Cert/License No</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Expiration Date (MM/DD/YYYY)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>haha</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>haha</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>08/22/2025</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>123215</t>
         </is>
       </c>
     </row>
@@ -1136,7 +2197,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1152,29 +2213,131 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Date Recorded (MM/DD/YYYY)</t>
+          <t>Year Established</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Direct Community Jobs</t>
+          <t>Form of Organization</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Direct Home Based</t>
+          <t>Specify Franchise</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Indirect Home Based</t>
+          <t>Major Activity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Direct Jobs Sustained</t>
-        </is>
-      </c>
+          <t>Minor Activity</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PSIC Group</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>PSIC Division</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>PSIC Section</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Prio Industry Cluster</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Trade Association and Affiliation</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Level of Business Operation Date (MM/DD/YYYY)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Growth Tracker</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>EDT Level</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Assisted By</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2028</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Sole Proprietorship</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Service</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>491</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Abaca and Abaca Products</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1187,7 +2350,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,67 +2366,39 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>EDT Assistance Level</t>
+          <t>Year Import Started</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Type of Assistance</t>
+          <t>Product Service</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Sub Type of Asisstance</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Remarks</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Date Start (MM/DD/YYYY)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Date End (MM/DD/YYYY)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>MSME Program</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>MSME Availed (MM/DD/YYYY)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Assisted By</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Assisting Office</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Assisting Officer Region</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Assisting Officer Province</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Assisting Officer City</t>
+          <t>Country</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ghahs</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>hashah</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add Excel download functionality and redesign Business Owner form
- Added 'Save Excel File' button in sidebar with timestamped filenames
- Redesigned Business Owner form with sectioned layout (Required vs Optional fields)
- Added visual hierarchy with red asterisks for required fields
- Implemented column mismatch error handling for DataFrame creation
- Enhanced form organization with clear field groupings
- Fixed data structure validation issues

Features:
- Excel file download with current date/time in filename
- Professional form layout with Required/Optional sections
- Robust error handling for data inconsistencies
- Improved user experience with clear visual indicators
</commit_message>
<xml_diff>
--- a/data/cpms_data.xlsx
+++ b/data/cpms_data.xlsx
@@ -648,11 +648,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>09/17/2024</t>
@@ -663,6 +663,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -673,6 +674,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
           <t>No</t>
@@ -688,6 +690,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -698,11 +702,13 @@
           <t>CRISTINA</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
           <t>MAGLASANG</t>
         </is>
       </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
           <t>Married</t>
@@ -713,6 +719,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr">
         <is>
           <t>centro</t>
@@ -723,26 +737,34 @@
           <t>1st</t>
         </is>
       </c>
+      <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="inlineStr">
         <is>
           <t>14 ST JUDE STREET, JEROME</t>
         </is>
       </c>
-      <c r="AJ2" t="n">
-        <v>9368188226</v>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>9368188226</t>
+        </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
           <t>carriemaglasang@gmail.com</t>
         </is>
       </c>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>09/19/2024</t>
@@ -753,6 +775,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -763,6 +786,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
           <t>No</t>
@@ -778,6 +802,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -788,11 +814,13 @@
           <t>IMELDA</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
           <t>RAÑOA</t>
         </is>
       </c>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
           <t>Married</t>
@@ -803,6 +831,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr">
         <is>
           <t>TORIL</t>
@@ -813,26 +849,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr">
         <is>
           <t xml:space="preserve"> LOT 23 BLOCK 48 RASAY</t>
         </is>
       </c>
-      <c r="AJ3" t="n">
-        <v>9177989922</v>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>9177989922</t>
+        </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
           <t>verdidaranoabuilding@gmail.com</t>
         </is>
       </c>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>09/20/2025</t>
@@ -843,6 +887,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -853,6 +898,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>No</t>
@@ -868,6 +914,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -878,11 +926,13 @@
           <t>MA. ILAISA</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
           <t>BRIONES</t>
         </is>
       </c>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr">
         <is>
           <t>Married</t>
@@ -893,6 +943,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr">
         <is>
           <t>9-A</t>
@@ -903,26 +961,34 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="inlineStr">
         <is>
           <t>door 2c mapa mabini complex</t>
         </is>
       </c>
-      <c r="AJ4" t="n">
-        <v>9982280722</v>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>9982280722</t>
+        </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
           <t>ilaidehcio@gmail.com</t>
         </is>
       </c>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>09/20/2025</t>
@@ -933,6 +999,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -943,6 +1010,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
           <t>No</t>
@@ -958,6 +1026,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -968,11 +1038,13 @@
           <t>RONITO</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
           <t>SIATON</t>
         </is>
       </c>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
         <is>
           <t>Married</t>
@@ -983,6 +1055,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
       <c r="AD5" t="inlineStr">
         <is>
           <t>CATALUNA PEQUEñO</t>
@@ -993,26 +1073,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="inlineStr">
         <is>
           <t>BLK 14 LOT 7 PHS 3 TUDAYA ST. WELLSPRING VILLAGE</t>
         </is>
       </c>
-      <c r="AJ5" t="n">
-        <v>9075354466</v>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>9075354466</t>
+        </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
           <t>ronitosiaton20@gmail.com</t>
         </is>
       </c>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>09/20/2025</t>
@@ -1023,6 +1111,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1033,6 +1122,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>No</t>
@@ -1048,6 +1138,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1058,11 +1150,13 @@
           <t>MELISSA</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr">
         <is>
           <t>BARING</t>
         </is>
       </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr">
         <is>
           <t>Married</t>
@@ -1073,6 +1167,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="inlineStr">
         <is>
           <t>ALFON ANGLIONTO SR.</t>
@@ -1083,26 +1185,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr">
         <is>
           <t>DAMOSA MARKET BASKET ANGLIONGTO AVEUE</t>
         </is>
       </c>
-      <c r="AJ6" t="n">
-        <v>9225948553</v>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>9225948553</t>
+        </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
           <t>dalmanginalyn@gmail.com</t>
         </is>
       </c>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>09/20/2025</t>
@@ -1113,6 +1223,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1123,6 +1234,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>No</t>
@@ -1138,6 +1250,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1148,11 +1262,13 @@
           <t>KRISTAL</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
           <t>PASAMBA</t>
         </is>
       </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr">
         <is>
           <t>Married</t>
@@ -1163,6 +1279,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr">
         <is>
           <t>MATINA CROSSING</t>
@@ -1173,26 +1297,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr">
         <is>
           <t>door 1&amp;2 nabua bldg matina aplaya road</t>
         </is>
       </c>
-      <c r="AJ7" t="n">
-        <v>9177700434</v>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>9177700434</t>
+        </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
           <t>kristalhuevos@gmail.com</t>
         </is>
       </c>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>09/20/2025</t>
@@ -1203,6 +1335,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1213,6 +1346,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
           <t>No</t>
@@ -1228,6 +1362,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1238,11 +1374,13 @@
           <t>RICHARD</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
           <t>BALLEGA</t>
         </is>
       </c>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr">
         <is>
           <t>Married</t>
@@ -1253,6 +1391,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="inlineStr">
         <is>
           <t>ILANG</t>
@@ -1263,26 +1409,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr">
         <is>
           <t>PUROK 7 AMPARO HOMES</t>
         </is>
       </c>
-      <c r="AJ8" t="n">
-        <v>9178752541</v>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>9178752541</t>
+        </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
           <t>stellariechester@gmail.com</t>
         </is>
       </c>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>09/24/2025</t>
@@ -1293,6 +1447,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1303,6 +1458,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
           <t>No</t>
@@ -1318,6 +1474,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1328,11 +1486,13 @@
           <t>JENIEFER</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
           <t>MONTECALVO</t>
         </is>
       </c>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr">
         <is>
           <t>Married</t>
@@ -1343,6 +1503,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="inlineStr">
         <is>
           <t>AGDAO</t>
@@ -1353,26 +1521,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr">
         <is>
           <t>BLK 10 LOT 5 RUIZ VILLAGE</t>
         </is>
       </c>
-      <c r="AJ9" t="n">
-        <v>9918239208</v>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>9918239208</t>
+        </is>
       </c>
       <c r="AK9" t="inlineStr">
         <is>
           <t>jeniefer.l.montecalvo@gmail.com</t>
         </is>
       </c>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>09/24/2025</t>
@@ -1383,6 +1559,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1393,6 +1570,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
           <t>No</t>
@@ -1408,6 +1586,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1418,11 +1598,13 @@
           <t>RUBY MAY</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
         <is>
           <t>BARROQUILLO</t>
         </is>
       </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr">
         <is>
           <t>Married</t>
@@ -1433,6 +1615,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr">
         <is>
           <t>TACUNAN</t>
@@ -1443,26 +1633,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="inlineStr">
         <is>
           <t>blk 3 lot 30 phase 12 jasmin st., deca homes</t>
         </is>
       </c>
-      <c r="AJ10" t="n">
-        <v>9959051038</v>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>9959051038</t>
+        </is>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
           <t>almayline@yahoo.com</t>
         </is>
       </c>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>07/14/2024</t>
@@ -1473,6 +1671,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1483,6 +1682,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
           <t>No</t>
@@ -1498,6 +1698,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1508,11 +1710,13 @@
           <t>CORAZON</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr">
         <is>
           <t>JAMONER</t>
         </is>
       </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
           <t>WIDOWER</t>
@@ -1523,6 +1727,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr">
         <is>
           <t>ALFONSO ANGLIONGTO SR.</t>
@@ -1533,26 +1745,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="inlineStr">
         <is>
           <t>BLK 9 LOT 29 BONIFACIO</t>
         </is>
       </c>
-      <c r="AJ11" t="n">
-        <v>9923950361</v>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>9923950361</t>
+        </is>
       </c>
       <c r="AK11" t="inlineStr">
         <is>
           <t>hinuguinqueenie22@gmail.com</t>
         </is>
       </c>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>10/04/2019</t>
@@ -1563,6 +1783,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1573,6 +1794,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
           <t>No</t>
@@ -1588,6 +1810,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1598,11 +1822,13 @@
           <t>HARA CLAIRE</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
           <t>FORTOLAZO</t>
         </is>
       </c>
+      <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr">
         <is>
           <t>Single</t>
@@ -1613,6 +1839,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="inlineStr">
         <is>
           <t>MATINA APLAYA</t>
@@ -1623,26 +1857,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF12" t="inlineStr"/>
       <c r="AG12" t="inlineStr">
         <is>
           <t>DEL CARMEN ST.</t>
         </is>
       </c>
-      <c r="AJ12" t="n">
-        <v>9395747966</v>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr">
+        <is>
+          <t>9395747966</t>
+        </is>
       </c>
       <c r="AK12" t="inlineStr">
         <is>
           <t>LEXBOOKKEEPERPLUS@gmail.com</t>
         </is>
       </c>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>08/18/2021</t>
@@ -1653,6 +1895,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1663,6 +1906,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
           <t>No</t>
@@ -1678,6 +1922,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1688,11 +1934,13 @@
           <t>MICHAEL</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr">
         <is>
           <t>PENA</t>
         </is>
       </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
           <t>Single</t>
@@ -1703,6 +1951,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="inlineStr">
         <is>
           <t>CATALUNA GRANDE</t>
@@ -1713,26 +1969,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="inlineStr">
         <is>
           <t>DOOR 3 2ND FLOOR CHARLES AND JULIA BLDG.</t>
         </is>
       </c>
-      <c r="AJ13" t="n">
-        <v>9958541060</v>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>9958541060</t>
+        </is>
       </c>
       <c r="AK13" t="inlineStr">
         <is>
           <t>michael_pena@umindanao.edu.ph</t>
         </is>
       </c>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>12/03/2024</t>
@@ -1743,6 +2007,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1753,6 +2018,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
           <t>No</t>
@@ -1768,6 +2034,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1778,11 +2046,13 @@
           <t>LORIBEL</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
           <t>TANDING</t>
         </is>
       </c>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr">
         <is>
           <t>Single</t>
@@ -1793,6 +2063,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr">
         <is>
           <t>BAGO APLAYA</t>
@@ -1803,26 +2081,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF14" t="inlineStr"/>
       <c r="AG14" t="inlineStr">
         <is>
           <t>PUROK 16 VICTORIA HILLS</t>
         </is>
       </c>
-      <c r="AJ14" t="n">
-        <v>9087739674</v>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>9087739674</t>
+        </is>
       </c>
       <c r="AK14" t="inlineStr">
         <is>
           <t>loribeltanding@gmail.com</t>
         </is>
       </c>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>05/13/2024</t>
@@ -1833,6 +2119,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1843,6 +2130,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
           <t>No</t>
@@ -1858,6 +2146,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1868,11 +2158,13 @@
           <t>MARIA LUISA</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr">
         <is>
           <t>MANZO</t>
         </is>
       </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr">
         <is>
           <t>Single</t>
@@ -1883,6 +2175,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr">
         <is>
           <t>TIGATTO</t>
@@ -1893,26 +2193,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="inlineStr">
         <is>
           <t>B76, L38, OPAL ST. DECA HOMES-ESPERANZA</t>
         </is>
       </c>
-      <c r="AJ15" t="n">
-        <v>9261061411</v>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>9261061411</t>
+        </is>
       </c>
       <c r="AK15" t="inlineStr">
         <is>
           <t>mluispm@rocketmail.com</t>
         </is>
       </c>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>08/03/2021</t>
@@ -1923,6 +2231,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -1933,6 +2242,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
           <t>No</t>
@@ -1948,6 +2258,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -1958,11 +2270,13 @@
           <t>LORENA</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
           <t>gracia</t>
         </is>
       </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
           <t>Married</t>
@@ -1973,6 +2287,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr">
         <is>
           <t>MAA</t>
@@ -1983,26 +2305,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="inlineStr">
         <is>
           <t xml:space="preserve"> PUROK 31, DOOR 2 DEL PILAR VIL.</t>
         </is>
       </c>
-      <c r="AJ16" t="n">
-        <v>9156871021</v>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>9156871021</t>
+        </is>
       </c>
       <c r="AK16" t="inlineStr">
         <is>
           <t>lorenabalaobao@gmail.com</t>
         </is>
       </c>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
           <t>01/10/2024</t>
@@ -2013,6 +2343,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2023,6 +2354,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
           <t>No</t>
@@ -2038,6 +2370,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2048,11 +2382,13 @@
           <t>ANN LOREEN</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr">
         <is>
           <t>OH</t>
         </is>
       </c>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr">
         <is>
           <t>Married</t>
@@ -2063,6 +2399,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="inlineStr">
         <is>
           <t>15-B</t>
@@ -2073,26 +2417,34 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF17" t="inlineStr"/>
       <c r="AG17" t="inlineStr">
         <is>
           <t>42 CERVANTES</t>
         </is>
       </c>
-      <c r="AJ17" t="n">
-        <v>9173011088</v>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>9173011088</t>
+        </is>
       </c>
       <c r="AK17" t="inlineStr">
         <is>
           <t>annloreen.lam@gmail.com</t>
         </is>
       </c>
+      <c r="AL17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
           <t>01/10/2024</t>
@@ -2103,6 +2455,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2113,6 +2466,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
           <t>No</t>
@@ -2128,6 +2482,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2138,11 +2494,13 @@
           <t>APRILLE JOY</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr">
         <is>
           <t>DELA CRUZ</t>
         </is>
       </c>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr">
         <is>
           <t>Single</t>
@@ -2153,6 +2511,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="inlineStr">
         <is>
           <t>SASA</t>
@@ -2163,26 +2529,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF18" t="inlineStr"/>
       <c r="AG18" t="inlineStr">
         <is>
           <t>106 DAISY ST</t>
         </is>
       </c>
-      <c r="AJ18" t="n">
-        <v>9162420036</v>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>9162420036</t>
+        </is>
       </c>
       <c r="AK18" t="inlineStr">
         <is>
           <t>lovely_aprille@yahoo.com</t>
         </is>
       </c>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
           <t>12/202/2019</t>
@@ -2193,6 +2567,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2203,6 +2578,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
           <t>No</t>
@@ -2218,6 +2594,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2228,11 +2606,13 @@
           <t>ARNALDO</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr">
         <is>
           <t>SAMONTE</t>
         </is>
       </c>
+      <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr">
         <is>
           <t>Married</t>
@@ -2243,6 +2623,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
       <c r="AD19" t="inlineStr">
         <is>
           <t>CATALUNAN PEQUENO</t>
@@ -2253,26 +2641,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF19" t="inlineStr"/>
       <c r="AG19" t="inlineStr">
         <is>
           <t>BLK. 2 LOT 6 RESIDENCIA DEL RIO</t>
         </is>
       </c>
-      <c r="AJ19" t="n">
-        <v>9368097654</v>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>9368097654</t>
+        </is>
       </c>
       <c r="AK19" t="inlineStr">
         <is>
           <t>arnaldosamonte1959@gmail.com</t>
         </is>
       </c>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
           <t>02/10/2024</t>
@@ -2283,6 +2679,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2293,6 +2690,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
           <t>No</t>
@@ -2308,6 +2706,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2318,11 +2718,13 @@
           <t>MARYLOU</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr">
         <is>
           <t>CAYBOT</t>
         </is>
       </c>
+      <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr">
         <is>
           <t>Married</t>
@@ -2333,6 +2735,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="inlineStr">
         <is>
           <t>VICENTE HIZON</t>
@@ -2343,26 +2753,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF20" t="inlineStr"/>
       <c r="AG20" t="inlineStr">
         <is>
           <t>ZONE 2 LIZADA VILLAGE</t>
         </is>
       </c>
-      <c r="AJ20" t="n">
-        <v>9634393438</v>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>9634393438</t>
+        </is>
       </c>
       <c r="AK20" t="inlineStr">
         <is>
           <t>m9505699@gmail.com</t>
         </is>
       </c>
+      <c r="AL20" t="inlineStr"/>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2373,6 +2791,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2383,6 +2802,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
           <t>No</t>
@@ -2398,6 +2818,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2408,11 +2830,13 @@
           <t>MARITES</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr">
         <is>
           <t>NAMANG</t>
         </is>
       </c>
+      <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr">
         <is>
           <t>WIDOWER</t>
@@ -2423,6 +2847,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr">
         <is>
           <t>CABANTIAN</t>
@@ -2433,26 +2865,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF21" t="inlineStr"/>
       <c r="AG21" t="inlineStr">
         <is>
           <t>PHASE 3 SAN FRANCISCO CORNER SAN VICENTE ST. LAVERNA HILL SUBD.</t>
         </is>
       </c>
-      <c r="AJ21" t="n">
-        <v>9281908829</v>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr">
+        <is>
+          <t>9281908829</t>
+        </is>
       </c>
       <c r="AK21" t="inlineStr">
         <is>
           <t>gflippage@gmail.com</t>
         </is>
       </c>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2463,6 +2903,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2473,6 +2914,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
           <t>No</t>
@@ -2488,6 +2930,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2498,11 +2942,13 @@
           <t>TERESITA</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr">
         <is>
           <t>VILLARTE</t>
         </is>
       </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr">
         <is>
           <t>WIDOWER</t>
@@ -2513,6 +2959,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="inlineStr">
         <is>
           <t>MATINA APLAYA</t>
@@ -2523,21 +2977,30 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="inlineStr">
         <is>
           <t>754 STA. ANA AVENUE</t>
         </is>
       </c>
-      <c r="AJ22" t="n">
-        <v>9226553193</v>
-      </c>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="inlineStr">
+        <is>
+          <t>9226553193</t>
+        </is>
+      </c>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2548,6 +3011,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2558,6 +3022,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
           <t>No</t>
@@ -2573,6 +3038,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2583,11 +3050,13 @@
           <t>JOHNNY</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr">
         <is>
           <t>LIBOON</t>
         </is>
       </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr">
         <is>
           <t xml:space="preserve">LEGALLY SEPARATED </t>
@@ -2598,6 +3067,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr">
         <is>
           <t>BUHANGIN</t>
@@ -2608,26 +3085,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="inlineStr">
         <is>
           <t>519 SAMPAGUITA</t>
         </is>
       </c>
-      <c r="AJ23" t="n">
-        <v>9154643088</v>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr">
+        <is>
+          <t>9154643088</t>
+        </is>
       </c>
       <c r="AK23" t="inlineStr">
         <is>
           <t>johnnyliboon@gmail.com</t>
         </is>
       </c>
+      <c r="AL23" t="inlineStr"/>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2638,6 +3123,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2648,6 +3134,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
           <t>No</t>
@@ -2663,6 +3150,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2673,11 +3162,13 @@
           <t>ROWENA</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr">
         <is>
           <t>SABLAS</t>
         </is>
       </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr">
         <is>
           <t>Single</t>
@@ -2688,6 +3179,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr"/>
+      <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr">
         <is>
           <t>AGDAO</t>
@@ -2698,21 +3197,30 @@
           <t>3RD</t>
         </is>
       </c>
-      <c r="AJ24" t="n">
-        <v>9564679769</v>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
+      <c r="AI24" t="inlineStr"/>
+      <c r="AJ24" t="inlineStr">
+        <is>
+          <t>9564679769</t>
+        </is>
       </c>
       <c r="AK24" t="inlineStr">
         <is>
           <t>sablasrowena@yahoo.com</t>
         </is>
       </c>
+      <c r="AL24" t="inlineStr"/>
+      <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2723,6 +3231,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2733,6 +3242,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
           <t>No</t>
@@ -2748,6 +3258,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2758,11 +3270,13 @@
           <t>JURIZEL</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr">
         <is>
           <t>BARBAJO</t>
         </is>
       </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr">
         <is>
           <t>Single</t>
@@ -2773,6 +3287,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="inlineStr">
         <is>
           <t>19-B</t>
@@ -2783,26 +3305,34 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF25" t="inlineStr"/>
       <c r="AG25" t="inlineStr">
         <is>
           <t>NILE STREER</t>
         </is>
       </c>
-      <c r="AJ25" t="n">
-        <v>9383685204</v>
+      <c r="AH25" t="inlineStr"/>
+      <c r="AI25" t="inlineStr"/>
+      <c r="AJ25" t="inlineStr">
+        <is>
+          <t>9383685204</t>
+        </is>
       </c>
       <c r="AK25" t="inlineStr">
         <is>
           <t>jurizelb@gmail.com</t>
         </is>
       </c>
+      <c r="AL25" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
           <t>06/01/2030</t>
@@ -2813,6 +3343,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2823,6 +3354,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
           <t>No</t>
@@ -2838,6 +3370,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2848,11 +3382,13 @@
           <t>JANYFE PATERNA</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr">
         <is>
           <t>ADLAON</t>
         </is>
       </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr">
         <is>
           <t>Married</t>
@@ -2863,6 +3399,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
+      <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="inlineStr">
         <is>
           <t>BUCANA</t>
@@ -2873,26 +3417,34 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF26" t="inlineStr"/>
       <c r="AG26" t="inlineStr">
         <is>
           <t>PUROK 66 BLK 21 LOT 8 SANTA TERESITA ST. , SIR NEW MATINA</t>
         </is>
       </c>
-      <c r="AJ26" t="n">
-        <v>9630764376</v>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="inlineStr">
+        <is>
+          <t>9630764376</t>
+        </is>
       </c>
       <c r="AK26" t="inlineStr">
         <is>
           <t>janyfepaternaadlaon@gmail.com</t>
         </is>
       </c>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2903,6 +3455,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -2913,6 +3466,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
           <t>No</t>
@@ -2928,6 +3482,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -2938,11 +3494,13 @@
           <t>LAUNFUL</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr">
         <is>
           <t>LAROT</t>
         </is>
       </c>
+      <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr">
         <is>
           <t>Single</t>
@@ -2953,6 +3511,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr">
         <is>
           <t>BANGKAS HEIGHTS</t>
@@ -2963,26 +3529,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF27" t="inlineStr"/>
       <c r="AG27" t="inlineStr">
         <is>
           <t>17 QUEENS AVENUE ROYAL VALLEY BANGKAL BANGKAS HEIGHTS</t>
         </is>
       </c>
-      <c r="AJ27" t="n">
-        <v>9385993127</v>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="inlineStr">
+        <is>
+          <t>9385993127</t>
+        </is>
       </c>
       <c r="AK27" t="inlineStr">
         <is>
           <t>dondoncutadmalinaolarot@gmail.com</t>
         </is>
       </c>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
           <t>06/01/2025</t>
@@ -2993,6 +3567,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3003,6 +3578,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
           <t>No</t>
@@ -3018,6 +3594,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3028,11 +3606,13 @@
           <t>PETER</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr">
         <is>
           <t>MANGIGO</t>
         </is>
       </c>
+      <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr">
         <is>
           <t>Married</t>
@@ -3043,6 +3623,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
       <c r="AD28" t="inlineStr">
         <is>
           <t>31-D</t>
@@ -3053,21 +3641,30 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF28" t="inlineStr"/>
       <c r="AG28" t="inlineStr">
         <is>
           <t>PUROK 8-A BOULEVARD</t>
         </is>
       </c>
-      <c r="AJ28" t="n">
-        <v>9452044378</v>
-      </c>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t>9452044378</t>
+        </is>
+      </c>
+      <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
           <t>07/01/2025</t>
@@ -3078,6 +3675,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3088,6 +3686,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
           <t>No</t>
@@ -3103,6 +3702,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3113,11 +3714,13 @@
           <t>MARIVIC</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr">
         <is>
           <t>MONTOJO</t>
         </is>
       </c>
+      <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr">
         <is>
           <t>Widowed</t>
@@ -3128,6 +3731,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
       <c r="AD29" t="inlineStr">
         <is>
           <t>CABATIAN</t>
@@ -3138,26 +3749,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF29" t="inlineStr"/>
       <c r="AG29" t="inlineStr">
         <is>
           <t>BLK31 LOT2 PH1 CIUDAD DE ESPERANZA MANGOSTEEN STREET</t>
         </is>
       </c>
-      <c r="AJ29" t="n">
-        <v>9096324771</v>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="inlineStr">
+        <is>
+          <t>9096324771</t>
+        </is>
       </c>
       <c r="AK29" t="inlineStr">
         <is>
           <t>marivicmontojo32@gmail.com</t>
         </is>
       </c>
+      <c r="AL29" t="inlineStr"/>
+      <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
           <t>07/01/2025</t>
@@ -3168,6 +3787,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3178,6 +3798,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
           <t>No</t>
@@ -3193,6 +3814,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3203,11 +3826,13 @@
           <t>JOHNDI</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr">
         <is>
           <t>SALENDE</t>
         </is>
       </c>
+      <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr">
         <is>
           <t>Single</t>
@@ -3218,6 +3843,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
       <c r="AD30" t="inlineStr">
         <is>
           <t>2-A</t>
@@ -3228,26 +3861,34 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF30" t="inlineStr"/>
       <c r="AG30" t="inlineStr">
         <is>
           <t>MAGALLANES</t>
         </is>
       </c>
-      <c r="AJ30" t="n">
-        <v>9165133101</v>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>9165133101</t>
+        </is>
       </c>
       <c r="AK30" t="inlineStr">
         <is>
           <t>httpkalog13@gmail.com</t>
         </is>
       </c>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
           <t>07/01/2025</t>
@@ -3258,6 +3899,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3268,6 +3910,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
           <t>No</t>
@@ -3283,6 +3926,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3293,11 +3938,13 @@
           <t>DHARRYL JIE</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr">
         <is>
           <t>ALINGALAN</t>
         </is>
       </c>
+      <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr">
         <is>
           <t>Single</t>
@@ -3308,6 +3955,14 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr">
         <is>
           <t>BUNAWAN</t>
@@ -3318,26 +3973,34 @@
           <t>3RD</t>
         </is>
       </c>
+      <c r="AF31" t="inlineStr"/>
       <c r="AG31" t="inlineStr">
         <is>
           <t>PUROK 3 DEVINE MERCY SAN ISIDRI</t>
         </is>
       </c>
-      <c r="AJ31" t="n">
-        <v>9452085765</v>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr"/>
+      <c r="AJ31" t="inlineStr">
+        <is>
+          <t>9452085765</t>
+        </is>
       </c>
       <c r="AK31" t="inlineStr">
         <is>
           <t>dharryljiea@gmail.com</t>
         </is>
       </c>
+      <c r="AL31" t="inlineStr"/>
+      <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
           <t>07/01/2025</t>
@@ -3348,6 +4011,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3358,6 +4022,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
           <t>No</t>
@@ -3373,6 +4038,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3383,11 +4050,13 @@
           <t>JOSEPHINE</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr">
         <is>
           <t>SANCHEZ</t>
         </is>
       </c>
+      <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr">
         <is>
           <t>Single</t>
@@ -3398,6 +4067,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
       <c r="AD32" t="inlineStr">
         <is>
           <t>BUCANA</t>
@@ -3408,26 +4085,34 @@
           <t>1ST</t>
         </is>
       </c>
+      <c r="AF32" t="inlineStr"/>
       <c r="AG32" t="inlineStr">
         <is>
           <t>ALMOND ST. SANDAWA</t>
         </is>
       </c>
-      <c r="AJ32" t="n">
-        <v>9683965682</v>
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="inlineStr"/>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>9683965682</t>
+        </is>
       </c>
       <c r="AK32" t="inlineStr">
         <is>
           <t>amarahuy1@gmail.com</t>
         </is>
       </c>
+      <c r="AL32" t="inlineStr"/>
+      <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
           <t>08/01/2025</t>
@@ -3438,6 +4123,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3448,6 +4134,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
           <t>No</t>
@@ -3463,6 +4150,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3473,11 +4162,13 @@
           <t>SHELLA MARIE</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr">
         <is>
           <t>CEPE</t>
         </is>
       </c>
+      <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr">
         <is>
           <t>Single</t>
@@ -3488,6 +4179,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="inlineStr">
         <is>
           <t>TALOMO</t>
@@ -3498,21 +4197,30 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF33" t="inlineStr"/>
       <c r="AG33" t="inlineStr">
         <is>
           <t>62-A SANTOS MKTG SUBD.BANGKAL DAVAO CITY</t>
         </is>
       </c>
-      <c r="AJ33" t="n">
-        <v>9303448041</v>
-      </c>
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" t="inlineStr">
+        <is>
+          <t>9303448041</t>
+        </is>
+      </c>
+      <c r="AK33" t="inlineStr"/>
+      <c r="AL33" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
           <t>08/01/2025</t>
@@ -3523,6 +4231,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3533,6 +4242,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
           <t>No</t>
@@ -3548,6 +4258,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3558,11 +4270,13 @@
           <t>EMILY</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr">
         <is>
           <t>TAMAYO</t>
         </is>
       </c>
+      <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr">
         <is>
           <t>Married</t>
@@ -3573,6 +4287,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr"/>
+      <c r="AC34" t="inlineStr"/>
       <c r="AD34" t="inlineStr">
         <is>
           <t>CATALUNA PEQUEñO</t>
@@ -3583,26 +4305,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF34" t="inlineStr"/>
       <c r="AG34" t="inlineStr">
         <is>
           <t>B5 L6 GRANVILLE 1 COLLINSVILLE STREET</t>
         </is>
       </c>
-      <c r="AJ34" t="n">
-        <v>9683258907</v>
+      <c r="AH34" t="inlineStr"/>
+      <c r="AI34" t="inlineStr"/>
+      <c r="AJ34" t="inlineStr">
+        <is>
+          <t>9683258907</t>
+        </is>
       </c>
       <c r="AK34" t="inlineStr">
         <is>
           <t>emilyztamayo2012@gmail.com</t>
         </is>
       </c>
+      <c r="AL34" t="inlineStr"/>
+      <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
           <t>08/01/2025</t>
@@ -3613,6 +4343,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3623,6 +4354,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
           <t>No</t>
@@ -3638,6 +4370,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3648,11 +4382,13 @@
           <t>DONNA VINZEL</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr">
         <is>
           <t>OLANDAG</t>
         </is>
       </c>
+      <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr">
         <is>
           <t>Married</t>
@@ -3663,6 +4399,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr"/>
+      <c r="AC35" t="inlineStr"/>
       <c r="AD35" t="inlineStr">
         <is>
           <t>TORIL</t>
@@ -3673,26 +4417,34 @@
           <t>2ND</t>
         </is>
       </c>
+      <c r="AF35" t="inlineStr"/>
       <c r="AG35" t="inlineStr">
         <is>
           <t>IVR BUILDING DOOR 3 RASAY STREET, TORIL,DAVAO CITY,DAVAO DEL SUR</t>
         </is>
       </c>
-      <c r="AJ35" t="n">
-        <v>9359317931</v>
+      <c r="AH35" t="inlineStr"/>
+      <c r="AI35" t="inlineStr"/>
+      <c r="AJ35" t="inlineStr">
+        <is>
+          <t>9359317931</t>
+        </is>
       </c>
       <c r="AK35" t="inlineStr">
         <is>
           <t>donnavinzelbautista@gmail.com</t>
         </is>
       </c>
+      <c r="AL35" t="inlineStr"/>
+      <c r="AM35" t="inlineStr"/>
+      <c r="AN35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
           <t>08/01/2025</t>
@@ -3703,6 +4455,7 @@
           <t>Level 2 - Growing Enterprises (Registered)</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
           <t>Self-Employed</t>
@@ -3713,6 +4466,7 @@
           <t>Abled</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
         <is>
           <t>No</t>
@@ -3728,6 +4482,8 @@
           <t>Level 2 (Intermediate) - MSMEs that have an online presence</t>
         </is>
       </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
           <t>Owner</t>
@@ -3738,11 +4494,13 @@
           <t>JEANEFER</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr">
         <is>
           <t>POLICIANOS</t>
         </is>
       </c>
+      <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr">
         <is>
           <t>Single</t>
@@ -3753,6 +4511,14 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
+      <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr"/>
+      <c r="AC36" t="inlineStr"/>
       <c r="AD36" t="inlineStr">
         <is>
           <t>talomo</t>
@@ -3763,19 +4529,27 @@
           <t>2nd</t>
         </is>
       </c>
+      <c r="AF36" t="inlineStr"/>
       <c r="AG36" t="inlineStr">
         <is>
           <t>PUROK 4 TALOMO SALAKOT</t>
         </is>
       </c>
-      <c r="AJ36" t="n">
-        <v>9815253244</v>
+      <c r="AH36" t="inlineStr"/>
+      <c r="AI36" t="inlineStr"/>
+      <c r="AJ36" t="inlineStr">
+        <is>
+          <t>9815253244</t>
+        </is>
       </c>
       <c r="AK36" t="inlineStr">
         <is>
           <t>policianosjeanefer1996@gmail.com</t>
         </is>
       </c>
+      <c r="AL36" t="inlineStr"/>
+      <c r="AM36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8639,17 +9413,6 @@
       <c r="E2" t="n">
         <v>6652587</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8675,17 +9438,6 @@
       <c r="E3" t="n">
         <v>6467093</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8711,17 +9463,6 @@
       <c r="E4" t="n">
         <v>5743605</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8747,17 +9488,6 @@
       <c r="E5" t="n">
         <v>2620554</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8783,17 +9513,6 @@
       <c r="E6" t="n">
         <v>6101811</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8819,17 +9538,6 @@
       <c r="E7" t="n">
         <v>4315136</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8855,17 +9563,6 @@
       <c r="E8" t="n">
         <v>5887170</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8891,17 +9588,6 @@
       <c r="E9" t="n">
         <v>5932800</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8927,17 +9613,6 @@
       <c r="E10" t="n">
         <v>1921584</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8963,17 +9638,6 @@
       <c r="E11" t="n">
         <v>6308782</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8999,17 +9663,6 @@
       <c r="E12" t="n">
         <v>6331138</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -9035,17 +9688,6 @@
       <c r="E13" t="n">
         <v>3190470</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -9071,17 +9713,6 @@
       <c r="E14" t="n">
         <v>5934997</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -9107,17 +9738,6 @@
       <c r="E15" t="n">
         <v>6145289</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -9143,17 +9763,6 @@
       <c r="E16" t="n">
         <v>2737113</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -9179,17 +9788,6 @@
       <c r="E17" t="n">
         <v>6653235</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -9215,17 +9813,6 @@
       <c r="E18" t="n">
         <v>6654530</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -9251,17 +9838,6 @@
       <c r="E19" t="n">
         <v>6493786</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -9287,17 +9863,6 @@
       <c r="E20" t="n">
         <v>6495333</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -9323,17 +9888,6 @@
       <c r="E21" t="n">
         <v>6655961</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -9341,21 +9895,6 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -9381,17 +9920,6 @@
       <c r="E23" t="n">
         <v>6657630</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -9417,17 +9945,6 @@
       <c r="E24" t="n">
         <v>6661187</v>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -9453,17 +9970,6 @@
       <c r="E25" t="n">
         <v>6661589</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -9489,17 +9995,6 @@
       <c r="E26" t="n">
         <v>6661702</v>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -9525,17 +10020,6 @@
       <c r="E27" t="n">
         <v>6661989</v>
       </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -9561,17 +10045,6 @@
       <c r="E28" t="n">
         <v>6664504</v>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -9597,17 +10070,6 @@
       <c r="E29" t="n">
         <v>6665334</v>
       </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -9633,17 +10095,6 @@
       <c r="E30" t="n">
         <v>6668176</v>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -9669,17 +10120,6 @@
       <c r="E31" t="n">
         <v>6670643</v>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -9705,17 +10145,6 @@
       <c r="E32" t="n">
         <v>5304024</v>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -9741,17 +10170,6 @@
       <c r="E33" t="n">
         <v>6317797</v>
       </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -9777,17 +10195,6 @@
       <c r="E34" t="n">
         <v>6679309</v>
       </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -9813,17 +10220,6 @@
       <c r="E35" t="n">
         <v>6680875</v>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -9849,17 +10245,6 @@
       <c r="E36" t="n">
         <v>6680994</v>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>